<commit_message>
canastas 2do sem 2020
</commit_message>
<xml_diff>
--- a/eph/canasta/canastas_eph.xlsx
+++ b/eph/canasta/canastas_eph.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="CBA" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,7 +56,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -78,12 +78,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,12 +121,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -143,6 +137,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -159,17 +157,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I51" activeCellId="0" sqref="I51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1625,6 +1623,162 @@
       </c>
       <c r="H56" s="2" t="n">
         <v>5997.44205</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>5929.29</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>5145.13</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>5289.67</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>5236.09</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>5838.43</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>6109.28</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>6081.69</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>5272.76</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>5432.89</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>5356.79</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>5981.63</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>6291.56</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>6288.17</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>5476.12</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>5632.44</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>5573.61</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>6214.79</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>6521.04</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>6702.33</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>5864.6</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>6014.33</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>5979.17</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>6671.74</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>6985.63</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>6981.61</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>6070.87</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>6239.72</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>6211.46</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>6937.09</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <v>7258.73</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>7340.12</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>6332.05</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>6575.43</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>6488.28</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>7267.36</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>7630.42</v>
       </c>
     </row>
   </sheetData>
@@ -1639,17 +1793,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H66" activeCellId="0" sqref="H66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J65" activeCellId="0" sqref="J65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3113,6 +3267,162 @@
       </c>
       <c r="H56" s="0" t="n">
         <v>2.76</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C61" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="G61" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C62" s="2" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>2.71</v>
       </c>
     </row>
   </sheetData>
@@ -3127,17 +3437,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I63" activeCellId="0" sqref="I63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4601,6 +4911,162 @@
       </c>
       <c r="H56" s="0" t="n">
         <v>16552.93</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>14408.17</v>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>11627.99</v>
+      </c>
+      <c r="E57" s="3" t="n">
+        <v>12060.45</v>
+      </c>
+      <c r="F57" s="3" t="n">
+        <v>13561.47</v>
+      </c>
+      <c r="G57" s="3" t="n">
+        <v>14187.38</v>
+      </c>
+      <c r="H57" s="3" t="n">
+        <v>16861.61</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C58" s="3" t="n">
+        <v>14717.69</v>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>11863.71</v>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>12332.66</v>
+      </c>
+      <c r="F58" s="3" t="n">
+        <v>13820.52</v>
+      </c>
+      <c r="G58" s="3" t="n">
+        <v>14475.54</v>
+      </c>
+      <c r="H58" s="3" t="n">
+        <v>17301.79</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C59" s="3" t="n">
+        <v>15280.25</v>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>12376.03</v>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>12841.96</v>
+      </c>
+      <c r="F59" s="3" t="n">
+        <v>14435.65</v>
+      </c>
+      <c r="G59" s="3" t="n">
+        <v>15101.94</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>17998.07</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C60" s="3" t="n">
+        <v>16152.62</v>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>13078.06</v>
+      </c>
+      <c r="E60" s="3" t="n">
+        <v>13532.24</v>
+      </c>
+      <c r="F60" s="3" t="n">
+        <v>15306.68</v>
+      </c>
+      <c r="G60" s="3" t="n">
+        <v>16078.89</v>
+      </c>
+      <c r="H60" s="3" t="n">
+        <v>19070.77</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C61" s="3" t="n">
+        <v>16755.86</v>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>13538.04</v>
+      </c>
+      <c r="E61" s="3" t="n">
+        <v>14039.37</v>
+      </c>
+      <c r="F61" s="3" t="n">
+        <v>15901.34</v>
+      </c>
+      <c r="G61" s="3" t="n">
+        <v>16649.02</v>
+      </c>
+      <c r="H61" s="3" t="n">
+        <v>19816.33</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C62" s="3" t="n">
+        <v>17542.89</v>
+      </c>
+      <c r="D62" s="3" t="n">
+        <v>14057.15</v>
+      </c>
+      <c r="E62" s="3" t="n">
+        <v>14728.96</v>
+      </c>
+      <c r="F62" s="3" t="n">
+        <v>16480.23</v>
+      </c>
+      <c r="G62" s="3" t="n">
+        <v>17368.99</v>
+      </c>
+      <c r="H62" s="3" t="n">
+        <v>20678.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>